<commit_message>
update topic for midterm day
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62C2488-279E-4642-BE39-43955FD769B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A68937-5D02-D144-B9D9-59776F585275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3D32A6EA-FFB9-A945-A00D-80F3A1F0AAB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>week</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Classes, interfaces, trees and tree traversals, SAT problem</t>
   </si>
   <si>
-    <t>Review on Wednesday, Midterm on Friday</t>
-  </si>
-  <si>
     <t>heuristics, graph representation, graph interface, graph traversal</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>GUI Output</t>
   </si>
   <si>
-    <t>Monday Review, Wednesday Midterm 2</t>
-  </si>
-  <si>
     <t>GUI Input, Event-driven programming, and MVC</t>
   </si>
   <si>
@@ -153,6 +147,9 @@
   </si>
   <si>
     <t>Thanksgiving recess November 28-December 1, 2024</t>
+  </si>
+  <si>
+    <t>Midterm on Wednesday</t>
   </si>
 </sst>
 </file>
@@ -530,7 +527,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +547,7 @@
         <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -564,7 +561,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -608,7 +605,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -619,7 +616,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -630,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -641,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -652,7 +649,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -663,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -674,7 +671,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -685,10 +682,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -699,7 +696,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -710,10 +707,10 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -724,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -735,7 +732,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed dates for first couple of weeks
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C797D896-9FBC-634C-8948-D902467176CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517C6318-AD56-194C-A445-F97B3B6103A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3D32A6EA-FFB9-A945-A00D-80F3A1F0AAB1}"/>
   </bookViews>
@@ -44,15 +44,6 @@
     <t>dates</t>
   </si>
   <si>
-    <t>Sep 11 - Sep 16</t>
-  </si>
-  <si>
-    <t>Sep 18 - Sep 23</t>
-  </si>
-  <si>
-    <t>Sep 25 - Sep 27</t>
-  </si>
-  <si>
     <t>Sep 30 - Oct 04</t>
   </si>
   <si>
@@ -140,10 +131,19 @@
     <t>Midterm on Wednesday</t>
   </si>
   <si>
-    <t>Aug 26 - Sept 09</t>
-  </si>
-  <si>
     <t>Java collections: arrays, lists, sets, and hashmaps and Algorithm patters: Sliding Window</t>
+  </si>
+  <si>
+    <t>Aug 26 - Sept 06</t>
+  </si>
+  <si>
+    <t>Sep 09 - Sep 13</t>
+  </si>
+  <si>
+    <t>Sep 16 - Sep 20</t>
+  </si>
+  <si>
+    <t>Sep 23 - Sep 27</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,10 +541,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,13 +552,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -588,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -599,10 +599,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -610,10 +610,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -621,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -632,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -643,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -654,10 +654,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,13 +665,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -679,10 +679,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,13 +690,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -704,10 +704,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -715,10 +715,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
moved midterms to correct weeks
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E05D9C-859B-4D4C-B946-83CE34386FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F54BFFE-D447-124D-9ADE-937EB78367B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3D32A6EA-FFB9-A945-A00D-80F3A1F0AAB1}"/>
   </bookViews>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,26 +583,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -649,26 +649,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>30</v>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
moved enum to week 9
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08930DCB-EFCE-7642-8795-094566CFE5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC9E333-7FED-D048-8F7F-3C200B6904D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3D32A6EA-FFB9-A945-A00D-80F3A1F0AAB1}"/>
   </bookViews>
@@ -92,9 +92,6 @@
     <t xml:space="preserve"> Inheritance, class hierarchies, debugging, using data to encode</t>
   </si>
   <si>
-    <t xml:space="preserve"> Interfaces, Object base class, enumerated types</t>
-  </si>
-  <si>
     <t>GUI Output</t>
   </si>
   <si>
@@ -140,10 +137,13 @@
     <t>Java collections: arrays, lists, sets, and hashmaps and Algorithm patterns: Sliding Window</t>
   </si>
   <si>
-    <t>Composing data structures, generics</t>
-  </si>
-  <si>
     <t>GUI principles</t>
+  </si>
+  <si>
+    <t>Object base class, Generics</t>
+  </si>
+  <si>
+    <t>Enumerated types, composing data structures</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,13 +552,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -588,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -668,10 +668,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -682,7 +682,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,10 +693,10 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added code smell to topics
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-210-website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6549835B-2BDA-EB46-BBF1-5815BAECBC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578EE246-8698-B04A-8606-512665C48082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{3D32A6EA-FFB9-A945-A00D-80F3A1F0AAB1}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Decomposition: top down and bottom up</t>
   </si>
   <si>
-    <t>Lambda functions</t>
-  </si>
-  <si>
     <t>holiday</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>review for final exam</t>
+  </si>
+  <si>
+    <t>Code Smells</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -552,13 +552,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -566,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,7 +577,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -588,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,7 +635,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -671,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -693,10 +693,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>